<commit_message>
:100:  Completed the Search by ID
</commit_message>
<xml_diff>
--- a/Project 2 Employee Temperature Infographics/HRProject_Temp_dummydata.xlsx
+++ b/Project 2 Employee Temperature Infographics/HRProject_Temp_dummydata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Araf\PycharmProjects\BasicPython\NesternShip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github Repos\Nesternship-BlueNes\Project 2 Employee Temperature Infographics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FECF3D3-5DE7-4AB1-A5D4-8E54D19DEC93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCA145C-A21E-42EB-BC47-EE49AE092DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="960" windowWidth="15375" windowHeight="7875" xr2:uid="{77F03ABE-A8D2-4667-88B4-3CE298A82CDB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77F03ABE-A8D2-4667-88B4-3CE298A82CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$3:$C$45</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="19">
   <si>
     <t>Personal Information</t>
   </si>
@@ -314,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,6 +344,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -693,11 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E6480F-4D9E-49D8-ADB0-B04D63B45B8F}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C45" sqref="C3:C45"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,36 +718,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="17" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="19" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -811,7 +813,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -843,7 +845,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -875,7 +877,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -907,7 +909,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -939,7 +941,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -1003,7 +1005,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -1035,7 +1037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -1067,7 +1069,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -1131,7 +1133,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>12</v>
       </c>
@@ -1195,7 +1197,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -1227,7 +1229,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -1259,7 +1261,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>16</v>
       </c>
@@ -1291,7 +1293,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>18</v>
       </c>
@@ -1387,7 +1389,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>20</v>
       </c>
@@ -1419,7 +1421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>21</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>22</v>
       </c>
@@ -1483,7 +1485,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>23</v>
       </c>
@@ -1515,7 +1517,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>24</v>
       </c>
@@ -1579,7 +1581,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>26</v>
       </c>
@@ -1611,7 +1613,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>27</v>
       </c>
@@ -1643,7 +1645,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>28</v>
       </c>
@@ -1675,7 +1677,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>29</v>
       </c>
@@ -1707,7 +1709,7 @@
         <v>36.9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>30</v>
       </c>
@@ -1771,7 +1773,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>32</v>
       </c>
@@ -1803,7 +1805,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>33</v>
       </c>
@@ -1835,7 +1837,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>34</v>
       </c>
@@ -1867,7 +1869,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>35</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>36</v>
       </c>
@@ -1963,7 +1965,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>38</v>
       </c>
@@ -1995,7 +1997,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>39</v>
       </c>
@@ -2027,7 +2029,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>40</v>
       </c>
@@ -2059,7 +2061,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>41</v>
       </c>
@@ -2091,7 +2093,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>42</v>
       </c>
@@ -2123,14 +2125,847 @@
         <v>37.700000000000003</v>
       </c>
     </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>43</v>
+      </c>
+      <c r="B46" s="5">
+        <v>88456287</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="J46" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>44</v>
+      </c>
+      <c r="B47" s="5">
+        <v>97352991</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="J47" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>45</v>
+      </c>
+      <c r="B48" s="5">
+        <v>28748821</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="1">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J48" s="1">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>46</v>
+      </c>
+      <c r="B49" s="5">
+        <v>94872843</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="1">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="J49" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>47</v>
+      </c>
+      <c r="B50" s="5">
+        <v>66387726</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="J50" s="1">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>48</v>
+      </c>
+      <c r="B51" s="11">
+        <v>11034485</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="J51" s="1">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>49</v>
+      </c>
+      <c r="B52" s="5">
+        <v>88456287</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="1">
+        <v>37.4</v>
+      </c>
+      <c r="J52" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>50</v>
+      </c>
+      <c r="B53" s="5">
+        <v>97352991</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="J53" s="1">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>51</v>
+      </c>
+      <c r="B54" s="5">
+        <v>28748821</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="1">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="J54" s="1">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>52</v>
+      </c>
+      <c r="B55" s="5">
+        <v>94872843</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" s="1">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="J55" s="1">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>53</v>
+      </c>
+      <c r="B56" s="5">
+        <v>66387726</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="1">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="J56" s="1">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
+        <v>54</v>
+      </c>
+      <c r="B57" s="11">
+        <v>11034485</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" s="1">
+        <v>38</v>
+      </c>
+      <c r="J57" s="1">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>55</v>
+      </c>
+      <c r="B58" s="5">
+        <v>88456287</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="1">
+        <v>37.4</v>
+      </c>
+      <c r="J58" s="1">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>56</v>
+      </c>
+      <c r="B59" s="5">
+        <v>97352991</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="J59" s="1">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>57</v>
+      </c>
+      <c r="B60" s="5">
+        <v>28748821</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="J60" s="1">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>58</v>
+      </c>
+      <c r="B61" s="5">
+        <v>94872843</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="J61" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>59</v>
+      </c>
+      <c r="B62" s="5">
+        <v>66387726</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="1">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="J62" s="1">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
+        <v>60</v>
+      </c>
+      <c r="B63" s="11">
+        <v>11034485</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="J63" s="1">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>61</v>
+      </c>
+      <c r="B64" s="5">
+        <v>88456287</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="1">
+        <v>37.9</v>
+      </c>
+      <c r="J64" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>62</v>
+      </c>
+      <c r="B65" s="5">
+        <v>97352991</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="J65" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>63</v>
+      </c>
+      <c r="B66" s="5">
+        <v>28748821</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G66" s="1">
+        <v>36.1</v>
+      </c>
+      <c r="J66" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>64</v>
+      </c>
+      <c r="B67" s="5">
+        <v>94872843</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G67" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="J67" s="1">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>65</v>
+      </c>
+      <c r="B68" s="5">
+        <v>66387726</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G68" s="1">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="J68" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="11">
+        <v>66</v>
+      </c>
+      <c r="B69" s="11">
+        <v>11034485</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G69" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="J69" s="1">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>67</v>
+      </c>
+      <c r="B70" s="5">
+        <v>88456287</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="J70" s="1">
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>68</v>
+      </c>
+      <c r="B71" s="5">
+        <v>97352991</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="J71" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>69</v>
+      </c>
+      <c r="B72" s="5">
+        <v>28748821</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="J72" s="1">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>70</v>
+      </c>
+      <c r="B73" s="5">
+        <v>94872843</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="J73" s="1">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>71</v>
+      </c>
+      <c r="B74" s="5">
+        <v>66387726</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G74" s="1">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J74" s="1">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="11">
+        <v>72</v>
+      </c>
+      <c r="B75" s="11">
+        <v>11034485</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="J75" s="1">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>73</v>
+      </c>
+      <c r="B76" s="5">
+        <v>88456287</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="J76" s="1">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>74</v>
+      </c>
+      <c r="B77" s="5">
+        <v>97352991</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="J77" s="1">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <v>75</v>
+      </c>
+      <c r="B78" s="5">
+        <v>28748821</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G78" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="J78" s="1">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
+        <v>76</v>
+      </c>
+      <c r="B79" s="5">
+        <v>94872843</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" s="1">
+        <v>36.6</v>
+      </c>
+      <c r="J79" s="1">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>77</v>
+      </c>
+      <c r="B80" s="5">
+        <v>66387726</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="J80" s="1">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="11">
+        <v>78</v>
+      </c>
+      <c r="B81" s="11">
+        <v>11034485</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G81" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="J81" s="1">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
+        <v>79</v>
+      </c>
+      <c r="B82" s="5">
+        <v>88456287</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="J82" s="1">
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>80</v>
+      </c>
+      <c r="B83" s="5">
+        <v>97352991</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G83" s="1">
+        <v>37.4</v>
+      </c>
+      <c r="J83" s="1">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>81</v>
+      </c>
+      <c r="B84" s="5">
+        <v>28748821</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="J84" s="1">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>82</v>
+      </c>
+      <c r="B85" s="5">
+        <v>94872843</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" s="1">
+        <v>37.9</v>
+      </c>
+      <c r="J85" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <v>83</v>
+      </c>
+      <c r="B86" s="5">
+        <v>66387726</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G86" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="J86" s="1">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="11">
+        <v>84</v>
+      </c>
+      <c r="B87" s="11">
+        <v>11034485</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G87" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="J87" s="1">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C3:C45" xr:uid="{7253B014-7F95-43DF-A7BA-505F0C761B9F}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Ayesha Mou"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="4">
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="E1:J1"/>

</xml_diff>